<commit_message>
changes made to fast and wrong
</commit_message>
<xml_diff>
--- a/swap curves.xlsx
+++ b/swap curves.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="118" documentId="8_{89156CCF-83EC-4B98-9701-714FF07C7AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA74AF67-11AD-4648-AE52-FD36DD63F065}"/>
   <bookViews>
-    <workbookView xWindow="-21420" yWindow="13065" windowWidth="20850" windowHeight="14400" activeTab="2" xr2:uid="{53304B67-2A9E-47DA-A394-3049710ED363}"/>
+    <workbookView xWindow="-21750" yWindow="12840" windowWidth="20850" windowHeight="14400" activeTab="1" xr2:uid="{53304B67-2A9E-47DA-A394-3049710ED363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2286,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1D147A-5431-4398-A9F5-A9D7E99DFD3E}">
   <dimension ref="B1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,6 +2396,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2403,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAD3480-2095-4661-B0EF-89DB84EE5B04}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>